<commit_message>
Increased cores, added a plea for real user stories.
</commit_message>
<xml_diff>
--- a/yarn/dd-yarn-tuning-guide.xlsx
+++ b/yarn/dd-yarn-tuning-guide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-5760" yWindow="-32000" windowWidth="45180" windowHeight="30580" tabRatio="288"/>
+    <workbookView xWindow="-4940" yWindow="-30280" windowWidth="39820" windowHeight="26020" tabRatio="288"/>
   </bookViews>
   <sheets>
     <sheet name="MapReduce Properties" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="109">
   <si>
     <t>Service</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Physical Memory and Virtual Cores</t>
   </si>
   <si>
-    <t>Default is 1028. Set to 0 when using Llama.</t>
-  </si>
-  <si>
     <t>Default is 1. Set to 0 when using Llama.</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
   </si>
   <si>
     <t>Default is 8.</t>
-  </si>
-  <si>
-    <t>Default is 64000.</t>
   </si>
   <si>
     <t>Default is 512.</t>
@@ -408,6 +402,27 @@
   </si>
   <si>
     <t>This is Work In Progress!</t>
+  </si>
+  <si>
+    <t>Default is 64,000.</t>
+  </si>
+  <si>
+    <t>Default is 1,028. Set to 0 when using Llama.</t>
+  </si>
+  <si>
+    <t>These machine specs are SWAGs based, in part,</t>
+  </si>
+  <si>
+    <t>on the examples in Admin training. It would be</t>
+  </si>
+  <si>
+    <t>great to hear some user stories and see some</t>
+  </si>
+  <si>
+    <t>configurations from the field that represent what</t>
+  </si>
+  <si>
+    <t>our customers are actually using.</t>
   </si>
 </sst>
 </file>
@@ -1576,17 +1591,7 @@
     <cellStyle name="Input" xfId="51" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2175,7 +2180,7 @@
   <dimension ref="B1:K25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I2" sqref="I2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2193,33 +2198,47 @@
   <sheetData>
     <row r="1" spans="2:11" ht="45">
       <c r="F1" s="120" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11">
+      <c r="I2" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:11">
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="19">
         <v>10</v>
       </c>
       <c r="D3" s="2"/>
+      <c r="I3" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" s="19">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="2"/>
       <c r="C5"/>
       <c r="D5" s="2"/>
+      <c r="I5" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="18">
       <c r="B6" s="111" t="s">
@@ -2228,13 +2247,16 @@
       <c r="C6" s="112"/>
       <c r="D6" s="112"/>
       <c r="E6" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -2249,11 +2271,11 @@
       </c>
       <c r="F7" s="101">
         <f>MIN(F10:F12)*$C$3</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G7" s="101">
         <f>MIN(G10:G12)*$C$3</f>
-        <v>80</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -2268,11 +2290,11 @@
       </c>
       <c r="F8" s="101">
         <f>MIN(F10:F12)*$C$3</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G8" s="101">
         <f>MIN(G10:G12)*$C$3</f>
-        <v>80</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="16">
@@ -2285,7 +2307,7 @@
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="113" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="113"/>
       <c r="D10" s="114"/>
@@ -2304,7 +2326,7 @@
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="113" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="113"/>
       <c r="D11" s="114"/>
@@ -2314,14 +2336,14 @@
       </c>
       <c r="F11" s="101">
         <f>'Resource Manager Properties'!E4/mapreduce.map.cpu.vcores</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G11" s="101">
         <f>'Resource Manager Properties'!F4/mapreduce.map.cpu.vcores</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="H11" s="119" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I11" s="119"/>
       <c r="J11" s="119"/>
@@ -2329,7 +2351,7 @@
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="113" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="113"/>
       <c r="D12" s="114"/>
@@ -2353,7 +2375,7 @@
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2597,7 +2619,7 @@
     <mergeCell ref="B12:D12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="K17 K23 K25 A2:J2 J6:J8 J13 E10:J12 I17 I18:K22 I23 I24:K24 I25 B13:H13 B6:H6 D15:J15 D16:K16 D17:E25 A15:C25 B3:B5 B9:J9 E7:H8 B7:B8 H3:J5 F3:G12 D3:D5 A3:A13 I1:J1 A1:G1">
+  <conditionalFormatting sqref="K17 K23 K25 A2:H2 J13 E10:J12 I17 I18:K22 I23 I24:K24 I25 B13:H13 B6:H6 D15:J15 D16:K16 D17:E25 A15:C25 B3:B5 B9:J9 E7:H8 B7:B8 H4:J5 F3:G12 D3:D5 A3:A13 A1:G1 J8 J2:J3 H3">
     <cfRule type="expression" dxfId="17" priority="2">
       <formula>CELL("protect",A1)=0</formula>
     </cfRule>
@@ -2625,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2645,7 +2667,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20">
       <c r="A1" s="80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -2666,21 +2688,21 @@
         <v>10</v>
       </c>
       <c r="D3" s="83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" s="83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F3" s="83" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="32">
       <c r="B4" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>13</v>
@@ -2691,20 +2713,20 @@
       </c>
       <c r="E4" s="79">
         <f>'DataNode Configurations'!$F$26</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F4" s="79">
         <f>'DataNode Configurations'!$F$40</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="48">
       <c r="B5" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>14</v>
@@ -2722,7 +2744,7 @@
         <v>216320</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" s="24"/>
     </row>
@@ -2741,21 +2763,21 @@
         <v>10</v>
       </c>
       <c r="D7" s="83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" s="83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="83" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
       <c r="B8" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>15</v>
@@ -2770,12 +2792,12 @@
         <v>1</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
       <c r="B9" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>16</v>
@@ -2786,19 +2808,19 @@
       </c>
       <c r="E9" s="79">
         <f>'DataNode Configurations'!$F$26</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F9" s="79">
         <f>'DataNode Configurations'!$F$40</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45">
       <c r="B10" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>17</v>
@@ -2831,21 +2853,21 @@
         <v>10</v>
       </c>
       <c r="D12" s="83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E12" s="83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F12" s="83" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30">
       <c r="B13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>18</v>
@@ -2860,12 +2882,12 @@
         <v>1028</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>20</v>
@@ -2883,12 +2905,12 @@
         <v>216320</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30">
       <c r="B15" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>21</v>
@@ -2903,7 +2925,7 @@
         <v>512</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2970,7 +2992,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2988,7 +3010,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="94" customFormat="1" ht="25">
       <c r="A1" s="90" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="91"/>
       <c r="C1" s="91"/>
@@ -3000,10 +3022,10 @@
     </row>
     <row r="2" spans="1:8" ht="18">
       <c r="A2" s="47" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>11</v>
@@ -3019,18 +3041,18 @@
         <v>2</v>
       </c>
       <c r="H2" s="87" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30">
       <c r="A3" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="62">
         <v>64</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="64" t="s">
@@ -3044,18 +3066,18 @@
         <v>12800</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="62">
         <v>12</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="64" t="s">
@@ -3069,22 +3091,22 @@
         <v>1024</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
       <c r="A5" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="62">
         <v>12</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="51">
         <v>0</v>
@@ -3094,18 +3116,18 @@
         <v>0</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="62">
         <v>2</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="63"/>
       <c r="E6" s="64" t="s">
@@ -3119,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
@@ -3138,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45">
@@ -3157,7 +3179,7 @@
         <v>6400</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
@@ -3175,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3218,7 +3240,7 @@
       <c r="C12" s="63"/>
       <c r="D12" s="63"/>
       <c r="E12" s="71" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" s="71">
         <f>cpu-SUM(F3:F11)</f>
@@ -3229,7 +3251,7 @@
         <v>43264</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" thickBot="1">
@@ -3257,7 +3279,7 @@
     </row>
     <row r="15" spans="1:8" s="94" customFormat="1" ht="25">
       <c r="A15" s="95" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="95"/>
       <c r="C15" s="95"/>
@@ -3269,10 +3291,10 @@
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="38" t="s">
         <v>11</v>
@@ -3288,18 +3310,18 @@
         <v>2</v>
       </c>
       <c r="H16" s="87" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30">
       <c r="A17" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="62">
         <v>96</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D17" s="67"/>
       <c r="E17" s="64" t="s">
@@ -3313,18 +3335,18 @@
         <v>19200</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" s="62">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18" s="67"/>
       <c r="E18" s="64" t="s">
@@ -3338,22 +3360,22 @@
         <v>1024</v>
       </c>
       <c r="H18" s="43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30">
       <c r="A19" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="62">
         <v>24</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19" s="67"/>
       <c r="E19" s="64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19" s="56">
         <v>0</v>
@@ -3363,18 +3385,18 @@
         <v>0</v>
       </c>
       <c r="H19" s="43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30">
       <c r="A20" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" s="62">
         <v>1</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20" s="67"/>
       <c r="E20" s="64" t="s">
@@ -3388,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30">
@@ -3407,7 +3429,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45">
@@ -3426,7 +3448,7 @@
         <v>9600</v>
       </c>
       <c r="H22" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30">
@@ -3444,7 +3466,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="43" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3487,18 +3509,18 @@
       <c r="C26" s="67"/>
       <c r="D26" s="68"/>
       <c r="E26" s="70" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" s="71">
         <f>cpu_2-SUM(F17:F25)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G26" s="65">
         <f>G27-SUM(G17:G25)</f>
         <v>66432</v>
       </c>
       <c r="H26" s="43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" thickBot="1">
@@ -3523,7 +3545,7 @@
     </row>
     <row r="29" spans="1:8" s="94" customFormat="1" ht="25">
       <c r="A29" s="98" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29" s="98"/>
       <c r="C29" s="98"/>
@@ -3535,10 +3557,10 @@
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>11</v>
@@ -3554,18 +3576,18 @@
         <v>2</v>
       </c>
       <c r="H30" s="39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30">
       <c r="A31" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" s="62">
         <v>256</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D31" s="67"/>
       <c r="E31" s="64" t="s">
@@ -3579,18 +3601,18 @@
         <v>19200</v>
       </c>
       <c r="H31" s="59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="62">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D32" s="67"/>
       <c r="E32" s="64" t="s">
@@ -3604,22 +3626,22 @@
         <v>1024</v>
       </c>
       <c r="H32" s="60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30">
       <c r="A33" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33" s="62">
         <v>24</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D33" s="67"/>
       <c r="E33" s="64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F33" s="51">
         <v>0</v>
@@ -3629,18 +3651,18 @@
         <v>0</v>
       </c>
       <c r="H33" s="60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30">
       <c r="A34" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" s="62">
         <v>1</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D34" s="67"/>
       <c r="E34" s="64" t="s">
@@ -3654,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30">
@@ -3673,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="45">
@@ -3692,7 +3714,7 @@
         <v>25600</v>
       </c>
       <c r="H36" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30">
@@ -3710,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="60" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -3752,18 +3774,18 @@
       <c r="C40" s="67"/>
       <c r="D40" s="68"/>
       <c r="E40" s="71" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F40" s="71">
         <f>cpu_3-SUM(F31:F39)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G40" s="65">
         <f>G41-SUM(G30:G37)</f>
         <v>216320</v>
       </c>
       <c r="H40" s="77" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Added names, corrected some formulae.
</commit_message>
<xml_diff>
--- a/yarn/dd-yarn-tuning-guide.xlsx
+++ b/yarn/dd-yarn-tuning-guide.xlsx
@@ -4,46 +4,56 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4940" yWindow="-30280" windowWidth="39820" windowHeight="26020" tabRatio="288"/>
+    <workbookView xWindow="1140" yWindow="-27580" windowWidth="39820" windowHeight="26020" tabRatio="288"/>
   </bookViews>
   <sheets>
     <sheet name="MapReduce Properties" sheetId="1" r:id="rId1"/>
-    <sheet name="Resource Manager Properties" sheetId="2" r:id="rId2"/>
-    <sheet name="DataNode Configurations" sheetId="4" r:id="rId3"/>
+    <sheet name="Master Node Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="Worker Node Configurations" sheetId="4" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="container_memory" localSheetId="2">'DataNode Configurations'!#REF!</definedName>
+    <definedName name="available_memory">'Worker Node Configurations'!$G$12</definedName>
+    <definedName name="available_memory2">'[1]Worker Node Configurations'!$G$26</definedName>
+    <definedName name="available_memory3">'[1]Worker Node Configurations'!$G$40</definedName>
+    <definedName name="available_vcores">'Worker Node Configurations'!$F$12</definedName>
+    <definedName name="available_vcores2">'Worker Node Configurations'!$F$26</definedName>
+    <definedName name="available_vcores3">'Worker Node Configurations'!$F$40</definedName>
+    <definedName name="container_memory" localSheetId="2">'Worker Node Configurations'!#REF!</definedName>
     <definedName name="container_memory">#REF!</definedName>
-    <definedName name="container_vcores" localSheetId="2">'DataNode Configurations'!#REF!</definedName>
+    <definedName name="container_vcores" localSheetId="2">'Worker Node Configurations'!#REF!</definedName>
     <definedName name="container_vcores">#REF!</definedName>
-    <definedName name="cpu" localSheetId="2">'DataNode Configurations'!$B$4</definedName>
+    <definedName name="cpu" localSheetId="2">'Worker Node Configurations'!$B$4</definedName>
     <definedName name="cpu">#REF!</definedName>
-    <definedName name="cpu_2">'DataNode Configurations'!$B$18</definedName>
-    <definedName name="cpu_3">'DataNode Configurations'!$B$32</definedName>
+    <definedName name="cpu_2">'Worker Node Configurations'!$B$18</definedName>
+    <definedName name="cpu_3">'Worker Node Configurations'!$B$32</definedName>
     <definedName name="CPU_Threads">'MapReduce Properties'!#REF!</definedName>
-    <definedName name="disks" localSheetId="2">'DataNode Configurations'!$B$5</definedName>
-    <definedName name="disks">#REF!</definedName>
-    <definedName name="mapreduce.map.cpu.vcores">'MapReduce Properties'!$J$19</definedName>
-    <definedName name="mapreduce.map.memory.mb">'MapReduce Properties'!$J$17</definedName>
-    <definedName name="mapreduce.reduce.cpu.vcores">'MapReduce Properties'!$J$22</definedName>
-    <definedName name="mapreduce.reduce.memory.mb">'MapReduce Properties'!$J$20</definedName>
-    <definedName name="nodes" localSheetId="2">'DataNode Configurations'!$B$42</definedName>
+    <definedName name="disks_1">'Worker Node Configurations'!$B$5</definedName>
+    <definedName name="disks_2">'Worker Node Configurations'!$B$19</definedName>
+    <definedName name="disks_3">'Worker Node Configurations'!$B$33</definedName>
+    <definedName name="mapreduce.map.cpu.vcores">'MapReduce Properties'!$J$20</definedName>
+    <definedName name="mapreduce.map.memory.mb">'MapReduce Properties'!$J$18</definedName>
+    <definedName name="mapreduce.reduce.cpu.vcores">'MapReduce Properties'!$J$23</definedName>
+    <definedName name="mapreduce.reduce.memory.mb">'MapReduce Properties'!$J$21</definedName>
+    <definedName name="nodes" localSheetId="2">'Worker Node Configurations'!$B$42</definedName>
     <definedName name="nodes">#REF!</definedName>
-    <definedName name="num_nodes" localSheetId="2">'DataNode Configurations'!$B$42</definedName>
+    <definedName name="num_nodes" localSheetId="2">'Worker Node Configurations'!$B$42</definedName>
     <definedName name="num_nodes">#REF!</definedName>
     <definedName name="Number_of_Nodes">'MapReduce Properties'!#REF!</definedName>
-    <definedName name="os_cores" localSheetId="2">'DataNode Configurations'!$F$3</definedName>
+    <definedName name="os_cores" localSheetId="2">'Worker Node Configurations'!$F$3</definedName>
     <definedName name="os_cores">#REF!</definedName>
     <definedName name="Other_CPU_Allocation">SUM('MapReduce Properties'!XEY1048563:XEY1048570)</definedName>
     <definedName name="Other_Mem_Allocation">'MapReduce Properties'!#REF!</definedName>
     <definedName name="Physical_Disks_per_Node">'MapReduce Properties'!#REF!</definedName>
-    <definedName name="ram" localSheetId="2">'DataNode Configurations'!$B$3</definedName>
+    <definedName name="ram" localSheetId="2">'Worker Node Configurations'!$B$3</definedName>
     <definedName name="ram">#REF!</definedName>
-    <definedName name="ram_2">'DataNode Configurations'!$B$17</definedName>
-    <definedName name="ram_3">'DataNode Configurations'!$B$31</definedName>
+    <definedName name="ram_2">'Worker Node Configurations'!$B$17</definedName>
+    <definedName name="ram_3">'Worker Node Configurations'!$B$31</definedName>
     <definedName name="RAM_on_each_Node">'MapReduce Properties'!#REF!</definedName>
     <definedName name="Workload_Factor">'MapReduce Properties'!$C$4</definedName>
-    <definedName name="yarn.app.mapreduce.am.resource.mb">'MapReduce Properties'!$J$23</definedName>
+    <definedName name="yarn.app.mapreduce.am.resource.mb">'MapReduce Properties'!$J$24</definedName>
     <definedName name="yarn.nodemanager.resource.cpuvcores">'MapReduce Properties'!#REF!</definedName>
     <definedName name="yarn.nodemanager.resource.memory">'MapReduce Properties'!#REF!</definedName>
     <definedName name="yarn.scheduler.minimumallocationvcores">'MapReduce Properties'!#REF!</definedName>
@@ -58,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
   <si>
     <t>Service</t>
   </si>
@@ -353,16 +363,10 @@
     <t>Very High</t>
   </si>
   <si>
-    <t>Resource and Node Manager Properties</t>
-  </si>
-  <si>
     <t>High-end - high memory, spindle dense 10GB Ethernet</t>
   </si>
   <si>
     <t>High-end - very high memory, spindle dense 10GB Ethernet</t>
-  </si>
-  <si>
-    <t>Available CPU cores</t>
   </si>
   <si>
     <t>Available disks</t>
@@ -423,6 +427,15 @@
   </si>
   <si>
     <t>our customers are actually using.</t>
+  </si>
+  <si>
+    <t>Available CPU cores (map)</t>
+  </si>
+  <si>
+    <t>Available CPU cores (reduce)</t>
+  </si>
+  <si>
+    <t>Master Node Properties</t>
   </si>
 </sst>
 </file>
@@ -904,7 +917,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -958,6 +971,10 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1412,7 +1429,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="50"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="181">
     <cellStyle name="Accent1" xfId="52" builtinId="29"/>
     <cellStyle name="Bad" xfId="50" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1502,6 +1519,8 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1588,10 +1607,62 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="51" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1850,6 +1921,34 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="MapReduce Properties"/>
+      <sheetName val="Master Node Properties"/>
+      <sheetName val="Worker Node Configurations"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="26">
+          <cell r="G26">
+            <v>66432</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="G40">
+            <v>216320</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2177,7 +2276,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K25"/>
+  <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:K6"/>
@@ -2198,12 +2297,12 @@
   <sheetData>
     <row r="1" spans="2:11" ht="45">
       <c r="F1" s="120" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="2:11">
       <c r="I2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="2:11">
@@ -2215,21 +2314,21 @@
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="19">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -2237,7 +2336,7 @@
       <c r="C5"/>
       <c r="D5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18">
@@ -2256,7 +2355,7 @@
         <v>90</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -2266,15 +2365,15 @@
       <c r="C7" s="116"/>
       <c r="D7" s="117"/>
       <c r="E7" s="101">
-        <f>MIN(E10:E12)*$C$3</f>
+        <f>MIN(E10:E13)*$C$3</f>
         <v>80</v>
       </c>
       <c r="F7" s="101">
-        <f>MIN(F10:F12)*$C$3</f>
+        <f>MIN(F10:F13)*$C$3</f>
         <v>120</v>
       </c>
       <c r="G7" s="101">
-        <f>MIN(G10:G12)*$C$3</f>
+        <f>MIN(G10:G13)*$C$3</f>
         <v>200</v>
       </c>
     </row>
@@ -2285,15 +2384,15 @@
       <c r="C8" s="116"/>
       <c r="D8" s="117"/>
       <c r="E8" s="101">
-        <f>MIN(E10:E12)*$C$3</f>
+        <f>MIN(E10:E13)*$C$3</f>
         <v>80</v>
       </c>
       <c r="F8" s="101">
-        <f>MIN(F10:F12)*$C$3</f>
+        <f>MIN(F10:F13)*$C$3</f>
         <v>120</v>
       </c>
       <c r="G8" s="101">
-        <f>MIN(G10:G12)*$C$3</f>
+        <f>MIN(G10:G13)*$C$3</f>
         <v>200</v>
       </c>
     </row>
@@ -2307,43 +2406,43 @@
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="113" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" s="113"/>
       <c r="D10" s="114"/>
       <c r="E10" s="101">
-        <f>ROUND('Resource Manager Properties'!D5/mapreduce.map.memory.mb,0)</f>
+        <f>ROUND(available_memory/mapreduce.map.memory.mb,0)</f>
         <v>42</v>
       </c>
       <c r="F10" s="101">
-        <f>ROUND('Resource Manager Properties'!E5/mapreduce.map.memory.mb,0)</f>
+        <f>ROUND(available_memory2/mapreduce.map.memory.mb,0)</f>
         <v>65</v>
       </c>
       <c r="G10" s="101">
-        <f>ROUND('Resource Manager Properties'!F5/mapreduce.map.memory.mb,0)</f>
+        <f>ROUND(available_memory3/mapreduce.map.memory.mb,0)</f>
         <v>211</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="113" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C11" s="113"/>
       <c r="D11" s="114"/>
       <c r="E11" s="101">
-        <f>'Resource Manager Properties'!D4/mapreduce.map.cpu.vcores</f>
+        <f>available_vcores/mapreduce.map.cpu.vcores</f>
         <v>8</v>
       </c>
       <c r="F11" s="101">
-        <f>'Resource Manager Properties'!E4/mapreduce.map.cpu.vcores</f>
+        <f>available_vcores2/mapreduce.map.cpu.vcores</f>
         <v>12</v>
       </c>
       <c r="G11" s="101">
-        <f>'Resource Manager Properties'!F4/mapreduce.map.cpu.vcores</f>
+        <f>available_vcores3/mapreduce.map.cpu.vcores</f>
         <v>20</v>
       </c>
       <c r="H11" s="119" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I11" s="119"/>
       <c r="J11" s="119"/>
@@ -2351,95 +2450,95 @@
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="113" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C12" s="113"/>
       <c r="D12" s="114"/>
       <c r="E12" s="101">
-        <f>'DataNode Configurations'!disks*Workload_Factor</f>
+        <f>available_vcores/mapreduce.reduce.cpu.vcores</f>
+        <v>8</v>
+      </c>
+      <c r="F12" s="101">
+        <f>available_vcores2/mapreduce.reduce.cpu.vcores</f>
+        <v>12</v>
+      </c>
+      <c r="G12" s="101">
+        <f>available_vcores3/mapreduce.reduce.cpu.vcores</f>
+        <v>20</v>
+      </c>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="113" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="113"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="101">
+        <f>disks_1*Workload_Factor</f>
         <v>24</v>
       </c>
-      <c r="F12" s="101">
-        <f>'DataNode Configurations'!disks*Workload_Factor</f>
-        <v>24</v>
-      </c>
-      <c r="G12" s="101">
-        <f>'DataNode Configurations'!disks*Workload_Factor</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="34"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="B15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" ht="18">
-      <c r="B16" s="13" t="s">
+      <c r="F13" s="101">
+        <f>disks_2*Workload_Factor</f>
+        <v>72</v>
+      </c>
+      <c r="G13" s="101">
+        <f>disks_3*Workload_Factor</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="34"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" ht="18">
+      <c r="B17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="102" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="103"/>
-      <c r="G16" s="104"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="4" t="s">
+      <c r="F17" s="103"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J17" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="18"/>
-    </row>
-    <row r="17" spans="2:11" ht="16" customHeight="1">
-      <c r="B17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="118" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="19">
-        <v>1024</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="2:11" ht="16" customHeight="1">
       <c r="B18" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
       <c r="E18" s="105" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="106"/>
       <c r="G18" s="106"/>
       <c r="H18" s="107"/>
       <c r="I18" s="118" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="3">
-        <f>ROUND(mapreduce.map.memory.mb*0.8,0)</f>
-        <v>819</v>
+        <v>19</v>
+      </c>
+      <c r="J18" s="19">
+        <v>1024</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>43</v>
@@ -2447,163 +2546,185 @@
     </row>
     <row r="19" spans="2:11" ht="16" customHeight="1">
       <c r="B19" s="14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="105" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F19" s="106"/>
       <c r="G19" s="106"/>
       <c r="H19" s="107"/>
-      <c r="I19" s="118">
-        <v>1</v>
-      </c>
-      <c r="J19" s="19">
-        <v>1</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>22</v>
+      <c r="I19" s="118" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="3">
+        <f>ROUND(mapreduce.map.memory.mb*0.8,0)</f>
+        <v>819</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="16" customHeight="1">
       <c r="B20" s="14" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
       <c r="E20" s="105" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="106"/>
       <c r="G20" s="106"/>
       <c r="H20" s="107"/>
-      <c r="I20" s="118" t="s">
-        <v>19</v>
+      <c r="I20" s="118">
+        <v>1</v>
       </c>
       <c r="J20" s="19">
-        <f>2*mapreduce.map.memory.mb</f>
-        <v>2048</v>
+        <v>1</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="16" customHeight="1">
       <c r="B21" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
       <c r="E21" s="105" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="106"/>
       <c r="G21" s="106"/>
       <c r="H21" s="107"/>
       <c r="I21" s="118" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="3">
-        <f>ROUND(mapreduce.reduce.memory.mb*0.8,0)</f>
-        <v>1638</v>
-      </c>
-      <c r="K21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="19">
+        <f>2*mapreduce.map.memory.mb</f>
+        <v>2048</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="16" customHeight="1">
       <c r="B22" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
       <c r="E22" s="105" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F22" s="106"/>
       <c r="G22" s="106"/>
       <c r="H22" s="107"/>
-      <c r="I22" s="118">
-        <v>1</v>
-      </c>
-      <c r="J22" s="19">
-        <v>1</v>
+      <c r="I22" s="118" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="3">
+        <f>ROUND(mapreduce.reduce.memory.mb*0.8,0)</f>
+        <v>1638</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="16" customHeight="1">
       <c r="B23" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
       <c r="E23" s="105" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F23" s="106"/>
       <c r="G23" s="106"/>
       <c r="H23" s="107"/>
-      <c r="I23" s="118" t="s">
-        <v>19</v>
+      <c r="I23" s="118">
+        <v>1</v>
       </c>
       <c r="J23" s="19">
-        <v>1024</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="50" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="16" customHeight="1">
       <c r="B24" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="108" t="s">
+      <c r="E24" s="105" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="106"/>
+      <c r="G24" s="106"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="19">
+        <v>1024</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="50" customHeight="1">
+      <c r="B25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="118" t="s">
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J25" s="3">
         <f>ROUND(yarn.app.mapreduce.am.resource.mb*0.8,0)</f>
         <v>819</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K25" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="16" customHeight="1">
-      <c r="B25" s="14" t="s">
+    <row r="26" spans="2:11" ht="16" customHeight="1">
+      <c r="B26" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="105" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="118">
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="118">
         <v>1</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J26" s="19">
         <v>1</v>
       </c>
-      <c r="K25" s="8"/>
+      <c r="K26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:H17"/>
+  <mergeCells count="16">
+    <mergeCell ref="J17:K17"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E19:H19"/>
     <mergeCell ref="E20:H20"/>
@@ -2611,24 +2732,31 @@
     <mergeCell ref="E22:H22"/>
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B12:D12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="K17 K23 K25 A2:H2 J13 E10:J12 I17 I18:K22 I23 I24:K24 I25 B13:H13 B6:H6 D15:J15 D16:K16 D17:E25 A15:C25 B3:B5 B9:J9 E7:H8 B7:B8 H4:J5 F3:G12 D3:D5 A3:A13 A1:G1 J8 J2:J3 H3">
-    <cfRule type="expression" dxfId="17" priority="2">
+  <conditionalFormatting sqref="K18 K24 K26 A2:H2 J14 I18 I19:K23 I24 I25:K25 I26 B14:H14 B6:H6 D16:J16 D17:K17 D18:E26 A16:C26 B3:B5 B9:J9 E7:H8 B7:B8 H4:J5 D3:D5 A3:A14 A1:G1 J8 J2:J3 H3 F3:G9 E13:J13 H10:J12">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>CELL("protect",A1)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J25">
+  <conditionalFormatting sqref="E10:G12">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>CELL("protect",E10)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26">
       <formula1>"1,2,4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17 J23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J18 J24">
       <formula1>"1024,2048,4096"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2647,9 +2775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2667,7 +2793,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20">
       <c r="A1" s="80" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -2708,15 +2834,15 @@
         <v>13</v>
       </c>
       <c r="D4" s="79">
-        <f>'DataNode Configurations'!$F$12</f>
+        <f>available_vcores</f>
         <v>8</v>
       </c>
       <c r="E4" s="79">
-        <f>'DataNode Configurations'!$F$26</f>
+        <f>available_vcores2</f>
         <v>12</v>
       </c>
       <c r="F4" s="79">
-        <f>'DataNode Configurations'!$F$40</f>
+        <f>available_vcores3</f>
         <v>20</v>
       </c>
       <c r="G4" s="28" t="s">
@@ -2732,15 +2858,15 @@
         <v>14</v>
       </c>
       <c r="D5" s="79">
-        <f>'DataNode Configurations'!$G$12</f>
+        <f>available_memory</f>
         <v>43264</v>
       </c>
       <c r="E5" s="79">
-        <f>'DataNode Configurations'!$G$26</f>
+        <f>available_memory2</f>
         <v>66432</v>
       </c>
       <c r="F5" s="79">
-        <f>'DataNode Configurations'!$G$40</f>
+        <f>available_memory3</f>
         <v>216320</v>
       </c>
       <c r="G5" s="28" t="s">
@@ -2803,15 +2929,15 @@
         <v>16</v>
       </c>
       <c r="D9" s="79">
-        <f>'DataNode Configurations'!$F$12</f>
+        <f>available_vcores</f>
         <v>8</v>
       </c>
       <c r="E9" s="79">
-        <f>'DataNode Configurations'!$F$26</f>
+        <f>available_vcores2</f>
         <v>12</v>
       </c>
       <c r="F9" s="79">
-        <f>'DataNode Configurations'!$F$40</f>
+        <f>available_vcores3</f>
         <v>20</v>
       </c>
       <c r="G9" s="20" t="s">
@@ -2882,7 +3008,7 @@
         <v>1028</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2893,19 +3019,19 @@
         <v>20</v>
       </c>
       <c r="D14" s="79">
-        <f>'DataNode Configurations'!$G$12</f>
+        <f>available_memory</f>
         <v>43264</v>
       </c>
       <c r="E14" s="79">
-        <f>'DataNode Configurations'!$G$26</f>
+        <f>available_memory2</f>
         <v>66432</v>
       </c>
       <c r="F14" s="79">
-        <f>'DataNode Configurations'!$G$40</f>
+        <f>available_memory3</f>
         <v>216320</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30">
@@ -2958,22 +3084,22 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:I5 G3 C3:F5 C7:G7 C12:G12">
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="21" priority="13">
       <formula>CELL("protect",C3)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="20" priority="6">
       <formula>CELL("protect",B4)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:F9">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>CELL("protect",D9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:F14">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>CELL("protect",D14)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2992,7 +3118,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3062,7 +3188,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="52">
-        <f>ram*'DataNode Configurations'!$F3*200</f>
+        <f>ram*'Worker Node Configurations'!$F3*200</f>
         <v>12800</v>
       </c>
       <c r="H3" s="43" t="s">
@@ -3087,7 +3213,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="52">
-        <f>'DataNode Configurations'!$F4*1024</f>
+        <f>'Worker Node Configurations'!$F4*1024</f>
         <v>1024</v>
       </c>
       <c r="H4" s="43" t="s">
@@ -3112,7 +3238,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="52">
-        <f>'DataNode Configurations'!$F5*16384</f>
+        <f>'Worker Node Configurations'!$F5*16384</f>
         <v>0</v>
       </c>
       <c r="H5" s="43" t="s">
@@ -3137,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="52">
-        <f>'DataNode Configurations'!$F6*16384</f>
+        <f>'Worker Node Configurations'!$F6*16384</f>
         <v>0</v>
       </c>
       <c r="H6" s="43" t="s">
@@ -3156,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="52">
-        <f>ram*'DataNode Configurations'!$F7*200</f>
+        <f>ram*'Worker Node Configurations'!$F7*200</f>
         <v>0</v>
       </c>
       <c r="H7" s="43" t="s">
@@ -3279,7 +3405,7 @@
     </row>
     <row r="15" spans="1:8" s="94" customFormat="1" ht="25">
       <c r="A15" s="95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="95"/>
       <c r="C15" s="95"/>
@@ -3356,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="46">
-        <f>'DataNode Configurations'!$F18*1024</f>
+        <f>'Worker Node Configurations'!$F18*1024</f>
         <v>1024</v>
       </c>
       <c r="H18" s="43" t="s">
@@ -3368,7 +3494,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="62">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>79</v>
@@ -3381,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="46">
-        <f>'DataNode Configurations'!$F19*16384</f>
+        <f>'Worker Node Configurations'!$F19*16384</f>
         <v>0</v>
       </c>
       <c r="H19" s="43" t="s">
@@ -3406,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="46">
-        <f>'DataNode Configurations'!$F20*16384</f>
+        <f>'Worker Node Configurations'!$F20*16384</f>
         <v>0</v>
       </c>
       <c r="H20" s="43" t="s">
@@ -3425,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="46">
-        <f>ram_2*'DataNode Configurations'!$F21*200</f>
+        <f>ram_2*'Worker Node Configurations'!$F21*200</f>
         <v>0</v>
       </c>
       <c r="H21" s="43" t="s">
@@ -3498,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="46">
-        <f>'DataNode Configurations'!$F25*1024</f>
+        <f>'Worker Node Configurations'!$F25*1024</f>
         <v>1024</v>
       </c>
       <c r="H25" s="43"/>
@@ -3545,7 +3671,7 @@
     </row>
     <row r="29" spans="1:8" s="94" customFormat="1" ht="25">
       <c r="A29" s="98" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="98"/>
       <c r="C29" s="98"/>
@@ -3634,7 +3760,7 @@
         <v>65</v>
       </c>
       <c r="B33" s="62">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C33" s="32" t="s">
         <v>79</v>
@@ -3812,67 +3938,67 @@
     <mergeCell ref="A29:C29"/>
   </mergeCells>
   <conditionalFormatting sqref="B17 B19:B20 B3:B14 G30 G32:G38 E2:G9 E25:F41 E24 G25:G28 E11:G23 E10">
-    <cfRule type="expression" dxfId="12" priority="17">
+    <cfRule type="expression" dxfId="17" priority="17">
       <formula>CELL("protect",B2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:C2">
-    <cfRule type="expression" dxfId="11" priority="16">
+    <cfRule type="expression" dxfId="16" priority="16">
       <formula>CELL("protect",A2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:C16">
-    <cfRule type="expression" dxfId="10" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>CELL("protect",A16)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="9" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>CELL("protect",B18)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31 B33:B34">
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>CELL("protect",B31)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:C30">
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>CELL("protect",A30)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>CELL("protect",B32)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:G41">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>CELL("protect",G40)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>CELL("protect",G31)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>CELL("protect",A1)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>CELL("protect",A29)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:G24">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>CELL("protect",F24)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:G10">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>CELL("protect",F10)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Some updates based on discussion 7/9/15
</commit_message>
<xml_diff>
--- a/yarn/dd-yarn-tuning-guide.xlsx
+++ b/yarn/dd-yarn-tuning-guide.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="-27580" windowWidth="39820" windowHeight="26020" tabRatio="288"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37720" windowHeight="19660" tabRatio="288"/>
   </bookViews>
   <sheets>
     <sheet name="MapReduce Properties" sheetId="1" r:id="rId1"/>
-    <sheet name="Master Node Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="YARN Configurations" sheetId="2" r:id="rId2"/>
     <sheet name="Worker Node Configurations" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
@@ -20,7 +20,7 @@
     <definedName name="available_memory3">'[1]Worker Node Configurations'!$G$40</definedName>
     <definedName name="available_vcores">'Worker Node Configurations'!$F$12</definedName>
     <definedName name="available_vcores2">'Worker Node Configurations'!$F$26</definedName>
-    <definedName name="available_vcores3">'Worker Node Configurations'!$F$40</definedName>
+    <definedName name="available_vcores3">'Worker Node Configurations'!$F$41</definedName>
     <definedName name="container_memory" localSheetId="2">'Worker Node Configurations'!#REF!</definedName>
     <definedName name="container_memory">#REF!</definedName>
     <definedName name="container_vcores" localSheetId="2">'Worker Node Configurations'!#REF!</definedName>
@@ -37,9 +37,9 @@
     <definedName name="mapreduce.map.memory.mb">'MapReduce Properties'!$J$18</definedName>
     <definedName name="mapreduce.reduce.cpu.vcores">'MapReduce Properties'!$J$23</definedName>
     <definedName name="mapreduce.reduce.memory.mb">'MapReduce Properties'!$J$21</definedName>
-    <definedName name="nodes" localSheetId="2">'Worker Node Configurations'!$B$42</definedName>
+    <definedName name="nodes" localSheetId="2">'Worker Node Configurations'!$B$44</definedName>
     <definedName name="nodes">#REF!</definedName>
-    <definedName name="num_nodes" localSheetId="2">'Worker Node Configurations'!$B$42</definedName>
+    <definedName name="num_nodes" localSheetId="2">'Worker Node Configurations'!$B$44</definedName>
     <definedName name="num_nodes">#REF!</definedName>
     <definedName name="Number_of_Nodes">'MapReduce Properties'!#REF!</definedName>
     <definedName name="os_cores" localSheetId="2">'Worker Node Configurations'!$F$3</definedName>
@@ -68,12 +68,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="113">
   <si>
     <t>Service</t>
-  </si>
-  <si>
-    <t>vcores</t>
   </si>
   <si>
     <t>Memory (MB)</t>
@@ -435,7 +432,19 @@
     <t>Available CPU cores (reduce)</t>
   </si>
   <si>
-    <t>Master Node Properties</t>
+    <t>8x8/core 2.9 GHz CPUs, 15 MB cache</t>
+  </si>
+  <si>
+    <t>Expected number of threads per core</t>
+  </si>
+  <si>
+    <t>Available cores</t>
+  </si>
+  <si>
+    <t>Total vcores</t>
+  </si>
+  <si>
+    <t>YARN Configurations</t>
   </si>
 </sst>
 </file>
@@ -917,7 +926,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1099,8 +1108,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1138,12 +1153,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="51"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1322,9 +1331,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="52" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="52" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="15" fillId="7" borderId="0" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1347,12 +1353,6 @@
     <xf numFmtId="3" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="18" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1362,17 +1362,11 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="16" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="52" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1384,6 +1378,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="50"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1402,10 +1413,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1414,22 +1428,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="50"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="52" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="16" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="18" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="52" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="51" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="187">
     <cellStyle name="Accent1" xfId="52" builtinId="29"/>
     <cellStyle name="Bad" xfId="50" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1521,6 +1539,9 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1609,10 +1630,13 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="51" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="23">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1842,38 +1866,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2276,10 +2268,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K26"/>
+  <dimension ref="B1:K31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K6"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2296,39 +2288,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="45">
-      <c r="F1" s="120" t="s">
-        <v>99</v>
+      <c r="F1" s="102" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="2:11">
       <c r="I2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:11">
       <c r="B3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="19">
+        <v>55</v>
+      </c>
+      <c r="C3" s="17">
         <v>10</v>
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="19">
+        <v>95</v>
+      </c>
+      <c r="C4" s="17">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -2336,419 +2328,421 @@
       <c r="C5"/>
       <c r="D5" s="2"/>
       <c r="I5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="I6" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="18">
-      <c r="B6" s="111" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="115" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="101">
-        <f>MIN(E10:E13)*$C$3</f>
-        <v>80</v>
-      </c>
-      <c r="F7" s="101">
-        <f>MIN(F10:F13)*$C$3</f>
-        <v>120</v>
-      </c>
-      <c r="G7" s="101">
-        <f>MIN(G10:G13)*$C$3</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="115" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="101">
-        <f>MIN(E10:E13)*$C$3</f>
-        <v>80</v>
-      </c>
-      <c r="F8" s="101">
-        <f>MIN(F10:F13)*$C$3</f>
-        <v>120</v>
-      </c>
-      <c r="G8" s="101">
-        <f>MIN(G10:G13)*$C$3</f>
-        <v>200</v>
-      </c>
-    </row>
     <row r="9" spans="2:11" ht="16">
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="113" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="101">
+      <c r="B10" s="114" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="114"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="94">
         <f>ROUND(available_memory/mapreduce.map.memory.mb,0)</f>
         <v>42</v>
       </c>
-      <c r="F10" s="101">
+      <c r="F10" s="94">
         <f>ROUND(available_memory2/mapreduce.map.memory.mb,0)</f>
         <v>65</v>
       </c>
-      <c r="G10" s="101">
+      <c r="G10" s="94">
         <f>ROUND(available_memory3/mapreduce.map.memory.mb,0)</f>
         <v>211</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="113" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="101">
+      <c r="B11" s="114" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="114"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="94">
         <f>available_vcores/mapreduce.map.cpu.vcores</f>
         <v>8</v>
       </c>
-      <c r="F11" s="101">
+      <c r="F11" s="94">
         <f>available_vcores2/mapreduce.map.cpu.vcores</f>
         <v>12</v>
       </c>
-      <c r="G11" s="101">
+      <c r="G11" s="94">
         <f>available_vcores3/mapreduce.map.cpu.vcores</f>
-        <v>20</v>
-      </c>
-      <c r="H11" s="119" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
+        <v>4</v>
+      </c>
+      <c r="H11" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="101"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="101"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="113" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="101">
+      <c r="B12" s="114" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="114"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="94">
         <f>available_vcores/mapreduce.reduce.cpu.vcores</f>
         <v>8</v>
       </c>
-      <c r="F12" s="101">
+      <c r="F12" s="94">
         <f>available_vcores2/mapreduce.reduce.cpu.vcores</f>
         <v>12</v>
       </c>
-      <c r="G12" s="101">
+      <c r="G12" s="94">
         <f>available_vcores3/mapreduce.reduce.cpu.vcores</f>
-        <v>20</v>
-      </c>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
+        <v>4</v>
+      </c>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="113" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="101">
+      <c r="B13" s="114" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="114"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="94">
         <f>disks_1*Workload_Factor</f>
         <v>24</v>
       </c>
-      <c r="F13" s="101">
+      <c r="F13" s="94">
         <f>disks_2*Workload_Factor</f>
         <v>72</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="94">
         <f>disks_3*Workload_Factor</f>
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="34"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:11" ht="18">
       <c r="B17" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="103"/>
-      <c r="G17" s="104"/>
+      <c r="E17" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="96"/>
+      <c r="G17" s="97"/>
       <c r="H17" s="11"/>
       <c r="I17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="J17" s="103" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" s="104"/>
     </row>
     <row r="18" spans="2:11" ht="16" customHeight="1">
       <c r="B18" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
       <c r="E18" s="105" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" s="106"/>
       <c r="G18" s="106"/>
       <c r="H18" s="107"/>
-      <c r="I18" s="118" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="19">
+      <c r="I18" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="17">
         <v>1024</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="16" customHeight="1">
       <c r="B19" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="105" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" s="106"/>
       <c r="G19" s="106"/>
       <c r="H19" s="107"/>
-      <c r="I19" s="118" t="s">
-        <v>29</v>
+      <c r="I19" s="100" t="s">
+        <v>28</v>
       </c>
       <c r="J19" s="3">
         <f>ROUND(mapreduce.map.memory.mb*0.8,0)</f>
         <v>819</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="16" customHeight="1">
       <c r="B20" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
       <c r="E20" s="105" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="106"/>
       <c r="G20" s="106"/>
       <c r="H20" s="107"/>
-      <c r="I20" s="118">
+      <c r="I20" s="100">
         <v>1</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="17">
         <v>1</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="16" customHeight="1">
       <c r="B21" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
       <c r="E21" s="105" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="106"/>
       <c r="G21" s="106"/>
       <c r="H21" s="107"/>
-      <c r="I21" s="118" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="19">
+      <c r="I21" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="17">
         <f>2*mapreduce.map.memory.mb</f>
         <v>2048</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="16" customHeight="1">
       <c r="B22" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
       <c r="E22" s="105" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="106"/>
       <c r="G22" s="106"/>
       <c r="H22" s="107"/>
-      <c r="I22" s="118" t="s">
-        <v>29</v>
+      <c r="I22" s="100" t="s">
+        <v>28</v>
       </c>
       <c r="J22" s="3">
         <f>ROUND(mapreduce.reduce.memory.mb*0.8,0)</f>
         <v>1638</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="16" customHeight="1">
       <c r="B23" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
       <c r="E23" s="105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="106"/>
       <c r="G23" s="106"/>
       <c r="H23" s="107"/>
-      <c r="I23" s="118">
+      <c r="I23" s="100">
         <v>1</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="17">
         <v>1</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="16" customHeight="1">
       <c r="B24" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
       <c r="E24" s="105" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="106"/>
       <c r="G24" s="106"/>
       <c r="H24" s="107"/>
-      <c r="I24" s="118" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="19">
+      <c r="I24" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="17">
         <v>1024</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="50" customHeight="1">
       <c r="B25" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
       <c r="E25" s="108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="109"/>
       <c r="G25" s="109"/>
       <c r="H25" s="110"/>
-      <c r="I25" s="118" t="s">
-        <v>29</v>
+      <c r="I25" s="100" t="s">
+        <v>28</v>
       </c>
       <c r="J25" s="3">
         <f>ROUND(yarn.app.mapreduce.am.resource.mb*0.8,0)</f>
         <v>819</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="16" customHeight="1">
       <c r="B26" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
       <c r="E26" s="105" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="106"/>
       <c r="G26" s="106"/>
       <c r="H26" s="107"/>
-      <c r="I26" s="118">
+      <c r="I26" s="100">
         <v>1</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="17">
         <v>1</v>
       </c>
       <c r="K26" s="8"/>
+    </row>
+    <row r="29" spans="2:11" ht="18">
+      <c r="B29" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="111" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="112"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="94">
+        <f>MIN(E10:E13)*$C$3</f>
+        <v>80</v>
+      </c>
+      <c r="F30" s="94">
+        <f>MIN(F10:F13)*$C$3</f>
+        <v>120</v>
+      </c>
+      <c r="G30" s="94">
+        <f>MIN(G10:G13)*$C$3</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="111" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="112"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="94">
+        <f>MIN(E10:E13)*$C$3</f>
+        <v>80</v>
+      </c>
+      <c r="F31" s="94">
+        <f>MIN(F10:F13)*$C$3</f>
+        <v>120</v>
+      </c>
+      <c r="G31" s="94">
+        <f>MIN(G10:G13)*$C$3</f>
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E19:H19"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="K18 K24 K26 A2:H2 J14 I18 I19:K23 I24 I25:K25 I26 B14:H14 B6:H6 D16:J16 D17:K17 D18:E26 A16:C26 B3:B5 B9:J9 E7:H8 B7:B8 H4:J5 D3:D5 A3:A14 A1:G1 J8 J2:J3 H3 F3:G9 E13:J13 H10:J12">
+  <conditionalFormatting sqref="K18 K24 K26 A2:H2 J14 I18 I19:K23 I24 I25:K25 I26 B14:H14 D16:J16 D17:K17 D18:E26 A16:C26 B3:B5 B30:B31 H4:J5 D3:D5 A3:A14 A1:G1 J8 J2:J3 H3 E13:J13 H10:J12 B29:G29 H6:H8 E30:G31 F3:G5 B9:J9 F29:G31">
     <cfRule type="expression" dxfId="22" priority="3">
       <formula>CELL("protect",A1)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:G12">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>CELL("protect",E10)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2775,308 +2769,310 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="44" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="44" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="25"/>
-    <col min="9" max="9" width="11" style="25" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="25"/>
+    <col min="1" max="1" width="3.5" style="23" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="42" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="42" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="23"/>
+    <col min="9" max="9" width="11" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="80"/>
+      <c r="A1" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="78"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1">
-      <c r="G2" s="25"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="83" t="s">
+      <c r="A3" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="116"/>
+      <c r="C3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="F3" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="32">
+      <c r="B4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="32">
-      <c r="B4" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="79">
+      <c r="C4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="77">
         <f>available_vcores</f>
         <v>8</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="77">
         <f>available_vcores2</f>
         <v>12</v>
       </c>
-      <c r="F4" s="79">
+      <c r="F4" s="77">
         <f>available_vcores3</f>
-        <v>20</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="24"/>
+        <v>4</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9" ht="48">
-      <c r="B5" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="79">
+      <c r="B5" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="77">
         <f>available_memory</f>
         <v>43264</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="77">
         <f>available_memory2</f>
         <v>66432</v>
       </c>
-      <c r="F5" s="79">
+      <c r="F5" s="77">
         <f>available_memory3</f>
         <v>216320</v>
       </c>
-      <c r="G5" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="24"/>
+      <c r="G5" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="25"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="83" t="s">
+      <c r="A7" s="116" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="116"/>
+      <c r="C7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>60</v>
+      <c r="F7" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="38">
+        <v>1</v>
+      </c>
+      <c r="E8" s="38">
+        <v>1</v>
+      </c>
+      <c r="F8" s="38">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
+      <c r="B9" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="40">
-        <v>1</v>
-      </c>
-      <c r="E8" s="40">
-        <v>1</v>
-      </c>
-      <c r="F8" s="40">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
-      <c r="B9" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="79">
+      <c r="D9" s="77">
         <f>available_vcores</f>
         <v>8</v>
       </c>
-      <c r="E9" s="79">
+      <c r="E9" s="77">
         <f>available_vcores2</f>
         <v>12</v>
       </c>
-      <c r="F9" s="79">
+      <c r="F9" s="77">
         <f>available_vcores3</f>
-        <v>20</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>52</v>
+        <v>4</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="38">
+        <v>1</v>
+      </c>
+      <c r="E10" s="38">
+        <v>1</v>
+      </c>
+      <c r="F10" s="38">
+        <v>1</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30">
+      <c r="B13" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="40">
-        <v>1</v>
-      </c>
-      <c r="E10" s="40">
-        <v>1</v>
-      </c>
-      <c r="F10" s="40">
-        <v>1</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30">
-      <c r="B13" s="21" t="s">
+      <c r="D13" s="38">
+        <v>1028</v>
+      </c>
+      <c r="E13" s="38">
+        <v>1028</v>
+      </c>
+      <c r="F13" s="38">
+        <v>1028</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="40">
-        <v>1028</v>
-      </c>
-      <c r="E13" s="40">
-        <v>1028</v>
-      </c>
-      <c r="F13" s="40">
-        <v>1028</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="B14" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="79">
+      <c r="C14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="77">
         <f>available_memory</f>
         <v>43264</v>
       </c>
-      <c r="E14" s="79">
+      <c r="E14" s="77">
         <f>available_memory2</f>
         <v>66432</v>
       </c>
-      <c r="F14" s="79">
+      <c r="F14" s="77">
         <f>available_memory3</f>
         <v>216320</v>
       </c>
-      <c r="G14" s="25" t="s">
-        <v>100</v>
+      <c r="G14" s="23" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30">
-      <c r="B15" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="40">
+      <c r="B15" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="38">
         <v>512</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="38">
         <v>512</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="38">
         <v>512</v>
       </c>
-      <c r="G15" s="25" t="s">
-        <v>54</v>
+      <c r="G15" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="G16" s="25"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="25"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="25"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="25"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="25"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="25"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="25"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="25"/>
+      <c r="G25" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3084,22 +3080,22 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:I5 G3 C3:F5 C7:G7 C12:G12">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>CELL("protect",C3)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>CELL("protect",B4)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:F9">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>CELL("protect",D9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:F14">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>CELL("protect",D14)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3115,821 +3111,850 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="25"/>
-    <col min="3" max="3" width="55.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="45" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="25" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="25"/>
+    <col min="1" max="1" width="27.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="23"/>
+    <col min="3" max="3" width="55.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="43" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="23" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="94" customFormat="1" ht="25">
-      <c r="A1" s="90" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="92"/>
+    <row r="1" spans="1:8" s="89" customFormat="1" ht="25">
+      <c r="A1" s="118" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="18">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="83"/>
+      <c r="E2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="84" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="60">
+        <v>64</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="50" t="s">
+      <c r="D3" s="61"/>
+      <c r="E3" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="49">
         <v>1</v>
       </c>
-      <c r="G2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="87" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30">
-      <c r="A3" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="62">
-        <v>64</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="51">
-        <v>1</v>
-      </c>
-      <c r="G3" s="52">
+      <c r="G3" s="50">
         <f>ram*'Worker Node Configurations'!$F3*200</f>
         <v>12800</v>
       </c>
-      <c r="H3" s="43" t="s">
-        <v>57</v>
+      <c r="H3" s="41" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="62">
+      <c r="A4" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="60">
         <v>12</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="51">
+      <c r="C4" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="49">
         <v>1</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="50">
         <f>'Worker Node Configurations'!$F4*1024</f>
         <v>1024</v>
       </c>
-      <c r="H4" s="43" t="s">
-        <v>59</v>
+      <c r="H4" s="41" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
-      <c r="A5" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="62">
+      <c r="A5" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="60">
         <v>12</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="51">
+      <c r="C5" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="49">
         <v>0</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="50">
         <f>'Worker Node Configurations'!$F5*16384</f>
         <v>0</v>
       </c>
-      <c r="H5" s="43" t="s">
-        <v>58</v>
+      <c r="H5" s="41" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="62">
+      <c r="A6" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="60">
         <v>2</v>
       </c>
-      <c r="C6" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="51">
+      <c r="C6" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="49">
         <v>0</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="50">
         <f>'Worker Node Configurations'!$F6*16384</f>
         <v>0</v>
       </c>
-      <c r="H6" s="43" t="s">
-        <v>61</v>
+      <c r="H6" s="41" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="51">
+      <c r="A7" s="61"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="49">
         <v>0</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="50">
         <f>ram*'Worker Node Configurations'!$F7*200</f>
         <v>0</v>
       </c>
-      <c r="H7" s="43" t="s">
-        <v>62</v>
+      <c r="H7" s="41" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="51">
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="49">
         <v>0</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="50">
         <f>ram*100</f>
         <v>6400</v>
       </c>
-      <c r="H8" s="60" t="s">
-        <v>77</v>
+      <c r="H8" s="58" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="51">
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="49">
         <v>0</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="51">
         <v>0</v>
       </c>
-      <c r="H9" s="43" t="s">
-        <v>75</v>
+      <c r="H9" s="41" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="19">
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="17">
         <v>1</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="71">
         <f>F10*1024</f>
         <v>1024</v>
       </c>
-      <c r="H10" s="43"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="63"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="54">
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="52">
         <v>1</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="50">
         <f>F11*1024</f>
         <v>1024</v>
       </c>
-      <c r="H11" s="43"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8" ht="46" thickBot="1">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="71">
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="69">
         <f>cpu-SUM(F3:F11)</f>
         <v>8</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="63">
         <f>G13-SUM(G3:G11)</f>
         <v>43264</v>
       </c>
-      <c r="H12" s="43" t="s">
-        <v>76</v>
+      <c r="H12" s="41" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" thickBot="1">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="78">
+      <c r="A13" s="61"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="76">
         <f>ram*1024</f>
         <v>65536</v>
       </c>
-      <c r="H13" s="66"/>
+      <c r="H13" s="64"/>
     </row>
     <row r="14" spans="1:8" ht="16">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
-    </row>
-    <row r="15" spans="1:8" s="94" customFormat="1" ht="25">
-      <c r="A15" s="95" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="95"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="97"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
+    </row>
+    <row r="15" spans="1:8" s="89" customFormat="1" ht="25">
+      <c r="A15" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="91"/>
     </row>
     <row r="16" spans="1:8" ht="18">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="83"/>
+      <c r="E16" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="84" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30">
+      <c r="A17" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="60">
+        <v>96</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="33" t="s">
+      <c r="D17" s="65"/>
+      <c r="E17" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="53">
         <v>1</v>
       </c>
-      <c r="G16" s="85" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="87" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30">
-      <c r="A17" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="62">
-        <v>96</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="55">
-        <v>1</v>
-      </c>
-      <c r="G17" s="46">
+      <c r="G17" s="44">
         <f>ram_2*200</f>
         <v>19200</v>
       </c>
-      <c r="H17" s="43" t="s">
-        <v>57</v>
+      <c r="H17" s="41" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="62">
+      <c r="A18" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="60">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="55">
+      <c r="C18" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="65"/>
+      <c r="E18" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="53">
         <v>1</v>
       </c>
-      <c r="G18" s="46">
+      <c r="G18" s="44">
         <f>'Worker Node Configurations'!$F18*1024</f>
         <v>1024</v>
       </c>
-      <c r="H18" s="43" t="s">
-        <v>59</v>
+      <c r="H18" s="41" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30">
-      <c r="A19" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="62">
+      <c r="A19" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="60">
         <v>36</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="56">
+      <c r="C19" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="65"/>
+      <c r="E19" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="54">
         <v>0</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="44">
         <f>'Worker Node Configurations'!$F19*16384</f>
         <v>0</v>
       </c>
-      <c r="H19" s="43" t="s">
-        <v>58</v>
+      <c r="H19" s="41" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30">
-      <c r="A20" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="62">
+      <c r="A20" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="60">
         <v>1</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="56">
+      <c r="C20" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="65"/>
+      <c r="E20" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="54">
         <v>0</v>
       </c>
-      <c r="G20" s="46">
+      <c r="G20" s="44">
         <f>'Worker Node Configurations'!$F20*16384</f>
         <v>0</v>
       </c>
-      <c r="H20" s="43" t="s">
-        <v>61</v>
+      <c r="H20" s="41" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30">
-      <c r="A21" s="67"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="56">
+      <c r="A21" s="65"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="54">
         <v>0</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="44">
         <f>ram_2*'Worker Node Configurations'!$F21*200</f>
         <v>0</v>
       </c>
-      <c r="H21" s="43" t="s">
-        <v>62</v>
+      <c r="H21" s="41" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="56">
+      <c r="A22" s="65"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="54">
         <v>0</v>
       </c>
-      <c r="G22" s="46">
+      <c r="G22" s="44">
         <f>ram_2*100</f>
         <v>9600</v>
       </c>
-      <c r="H22" s="60" t="s">
-        <v>77</v>
+      <c r="H22" s="58" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="56">
+      <c r="A23" s="65"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="54">
         <v>0</v>
       </c>
-      <c r="G23" s="69">
+      <c r="G23" s="67">
         <v>0</v>
       </c>
-      <c r="H23" s="43" t="s">
-        <v>75</v>
+      <c r="H23" s="41" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="19">
+      <c r="A24" s="65"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="17">
         <v>1</v>
       </c>
-      <c r="G24" s="73">
+      <c r="G24" s="71">
         <f>F24*1024</f>
         <v>1024</v>
       </c>
-      <c r="H24" s="43"/>
+      <c r="H24" s="41"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="55">
+      <c r="A25" s="65"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="53">
         <v>1</v>
       </c>
-      <c r="G25" s="46">
+      <c r="G25" s="44">
         <f>'Worker Node Configurations'!$F25*1024</f>
         <v>1024</v>
       </c>
-      <c r="H25" s="43"/>
+      <c r="H25" s="41"/>
     </row>
     <row r="26" spans="1:8" ht="46" thickBot="1">
-      <c r="A26" s="67"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="71">
+      <c r="A26" s="65"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="69">
         <f>cpu_2-SUM(F17:F25)</f>
         <v>12</v>
       </c>
-      <c r="G26" s="65">
+      <c r="G26" s="63">
         <f>G27-SUM(G17:G25)</f>
         <v>66432</v>
       </c>
-      <c r="H26" s="43" t="s">
-        <v>76</v>
+      <c r="H26" s="41" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" thickBot="1">
-      <c r="A27" s="67"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="78">
+      <c r="A27" s="65"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="76">
         <f>ram_2*1024</f>
         <v>98304</v>
       </c>
-      <c r="H27" s="66"/>
+      <c r="H27" s="64"/>
     </row>
     <row r="28" spans="1:8" ht="16">
-      <c r="D28" s="20"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="42"/>
-    </row>
-    <row r="29" spans="1:8" s="94" customFormat="1" ht="25">
-      <c r="A29" s="98" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="100"/>
-      <c r="H29" s="92"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="1:8" s="89" customFormat="1" ht="25">
+      <c r="A29" s="120" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="120"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="87"/>
     </row>
     <row r="30" spans="1:8" ht="18">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30">
+      <c r="A31" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="60">
+        <v>256</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30"/>
-      <c r="E30" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="31" t="s">
+      <c r="D31" s="65"/>
+      <c r="E31" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="52">
         <v>1</v>
       </c>
-      <c r="G30" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30">
-      <c r="A31" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="62">
-        <v>256</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="67"/>
-      <c r="E31" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="54">
-        <v>1</v>
-      </c>
-      <c r="G31" s="58">
+      <c r="G31" s="56">
         <f>ram_2*F31*200</f>
         <v>19200</v>
       </c>
-      <c r="H31" s="59" t="s">
-        <v>57</v>
+      <c r="H31" s="57" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="62">
-        <v>24</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="67"/>
-      <c r="E32" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="54">
+      <c r="A32" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="60">
+        <v>64</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="65"/>
+      <c r="E32" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="52">
         <v>1</v>
       </c>
-      <c r="G32" s="73">
+      <c r="G32" s="71">
         <f>F32*1024</f>
         <v>1024</v>
       </c>
-      <c r="H32" s="60" t="s">
-        <v>59</v>
+      <c r="H32" s="58" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30">
-      <c r="A33" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="62">
+      <c r="A33" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="60">
         <v>36</v>
       </c>
-      <c r="C33" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="67"/>
-      <c r="E33" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" s="51">
+      <c r="C33" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="65"/>
+      <c r="E33" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="49">
         <v>0</v>
       </c>
-      <c r="G33" s="73">
+      <c r="G33" s="71">
         <f>F33*16384</f>
         <v>0</v>
       </c>
-      <c r="H33" s="60" t="s">
-        <v>58</v>
+      <c r="H33" s="58" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30">
-      <c r="A34" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="62">
+      <c r="A34" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="60">
         <v>1</v>
       </c>
-      <c r="C34" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="67"/>
-      <c r="E34" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="51">
+      <c r="C34" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="65"/>
+      <c r="E34" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="49">
         <v>0</v>
       </c>
-      <c r="G34" s="73">
+      <c r="G34" s="71">
         <f>F34*16384</f>
         <v>0</v>
       </c>
-      <c r="H34" s="60" t="s">
-        <v>61</v>
+      <c r="H34" s="58" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30">
-      <c r="A35" s="67"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="51">
+      <c r="A35" s="65"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="49">
         <v>0</v>
       </c>
-      <c r="G35" s="73">
+      <c r="G35" s="71">
         <f>ram_3*F35*200</f>
         <v>0</v>
       </c>
-      <c r="H35" s="60" t="s">
-        <v>62</v>
+      <c r="H35" s="58" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="45">
-      <c r="A36" s="67"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="51">
+      <c r="A36" s="65"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="49">
         <v>0</v>
       </c>
-      <c r="G36" s="73">
+      <c r="G36" s="71">
         <f>ram_3*100</f>
         <v>25600</v>
       </c>
-      <c r="H36" s="60" t="s">
-        <v>77</v>
+      <c r="H36" s="58" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30">
-      <c r="A37" s="67"/>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="51">
+      <c r="A37" s="65"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="49">
         <v>0</v>
       </c>
-      <c r="G37" s="74">
+      <c r="G37" s="72">
         <v>0</v>
       </c>
-      <c r="H37" s="60" t="s">
-        <v>75</v>
+      <c r="H37" s="58" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="67"/>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="19">
+      <c r="A38" s="65"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="17">
         <v>1</v>
       </c>
-      <c r="G38" s="73">
+      <c r="G38" s="71">
         <f>F38*1024</f>
         <v>1024</v>
       </c>
-      <c r="H38" s="60"/>
+      <c r="H38" s="58"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="67"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="64" t="s">
+      <c r="A39" s="65"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="52">
+        <v>1</v>
+      </c>
+      <c r="G39" s="73">
+        <v>1024</v>
+      </c>
+      <c r="H39" s="59"/>
+    </row>
+    <row r="40" spans="1:8" ht="45">
+      <c r="A40" s="65"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="69">
+        <f>cpu_3-SUM(F31:F39)</f>
+        <v>60</v>
+      </c>
+      <c r="G40" s="63">
+        <f>G43-SUM(G31:G39)</f>
+        <v>214272</v>
+      </c>
+      <c r="H40" s="75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30">
+      <c r="A41" s="65"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="121">
         <v>4</v>
       </c>
-      <c r="F39" s="54">
-        <v>1</v>
-      </c>
-      <c r="G39" s="75">
-        <v>1024</v>
-      </c>
-      <c r="H39" s="61"/>
-    </row>
-    <row r="40" spans="1:8" ht="46" thickBot="1">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="71">
-        <f>cpu_3-SUM(F31:F39)</f>
-        <v>20</v>
-      </c>
-      <c r="G40" s="65">
-        <f>G41-SUM(G30:G37)</f>
-        <v>216320</v>
-      </c>
-      <c r="H40" s="77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="16" thickBot="1">
-      <c r="A41" s="67"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="78">
+      <c r="G41" s="63"/>
+      <c r="H41" s="75"/>
+    </row>
+    <row r="42" spans="1:8" ht="16" thickBot="1">
+      <c r="A42" s="65"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="70">
+        <f>F40*available_vcores3</f>
+        <v>240</v>
+      </c>
+      <c r="G42" s="77"/>
+      <c r="H42" s="74"/>
+    </row>
+    <row r="43" spans="1:8" ht="16" thickBot="1">
+      <c r="A43" s="65"/>
+      <c r="B43" s="65"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="76">
         <f>ram_3*1024</f>
         <v>262144</v>
       </c>
-      <c r="H41" s="76"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="E42" s="20"/>
-      <c r="G42" s="44"/>
+      <c r="H43" s="74"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="E44" s="18"/>
+      <c r="G44" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3937,69 +3962,79 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A29:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17 B19:B20 B3:B14 G30 G32:G38 E2:G9 E25:F41 E24 G25:G28 E11:G23 E10">
-    <cfRule type="expression" dxfId="17" priority="17">
+  <conditionalFormatting sqref="B17 B19:B20 B3:B14 G30 G32:G38 E2:G9 E25:F39 E24 G25:G28 E11:G23 E10 E41:F43">
+    <cfRule type="expression" dxfId="16" priority="19">
       <formula>CELL("protect",B2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:C2">
-    <cfRule type="expression" dxfId="16" priority="16">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>CELL("protect",A2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:C16">
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="14" priority="17">
       <formula>CELL("protect",A16)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>CELL("protect",B18)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31 B33:B34">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>CELL("protect",B31)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:C30">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>CELL("protect",A30)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>CELL("protect",B32)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40:G41">
-    <cfRule type="expression" dxfId="10" priority="6">
-      <formula>CELL("protect",G40)=0</formula>
+  <conditionalFormatting sqref="G41:G43">
+    <cfRule type="expression" dxfId="9" priority="8">
+      <formula>CELL("protect",G41)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>CELL("protect",G31)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>CELL("protect",A1)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>CELL("protect",A29)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:G24">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>CELL("protect",F24)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:G10">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>CELL("protect",F10)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40:F40">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>CELL("protect",E40)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>CELL("protect",G40)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>